<commit_message>
jumlah report rekap golongan (kurang monitoring dan ttd))
</commit_message>
<xml_diff>
--- a/templates/report/golongan.xlsx
+++ b/templates/report/golongan.xlsx
@@ -5,22 +5,30 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMD\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64new\www\mojokerto_simpeg\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1810A8-63A7-4368-B6D4-729A345DDA4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0CD046-ECBF-4273-A136-7FA94405E578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <r>
       <rPr>
@@ -253,8 +261,13 @@
     </r>
   </si>
   <si>
-    <t>REKAPITULASI JUMLAH PEGAWAI NEGERI SIPIL PEMERINTAH KABUPATEN MOJOKERTO  BERDASARKAN GOLONGAN
-KEADAAN SEMESTER II TAHUN 2023</t>
+    <t>REKAPITULASI JUMLAH PEGAWAI NEGERI SIPIL PEMERINTAH KABUPATEN MOJOKERTO</t>
+  </si>
+  <si>
+    <t>BERDASARKAN GOLONGAN</t>
+  </si>
+  <si>
+    <t>KEADAAN SEMESTER I TAHUN 2024</t>
   </si>
 </sst>
 </file>
@@ -300,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -330,33 +343,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -365,9 +352,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -378,16 +363,27 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -427,12 +423,12 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -443,16 +439,16 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,9 +472,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2157187</xdr:colOff>
+      <xdr:colOff>1004662</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>400050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="464491" cy="552450"/>
     <xdr:pic>
@@ -508,7 +504,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2461987" y="123825"/>
+          <a:off x="1309462" y="400050"/>
           <a:ext cx="464491" cy="552450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -842,18 +838,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" customWidth="1"/>
-    <col min="4" max="5" width="3.1640625" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" customWidth="1"/>
     <col min="6" max="6" width="3.5" customWidth="1"/>
     <col min="7" max="7" width="3.83203125" customWidth="1"/>
     <col min="8" max="8" width="3.5" customWidth="1"/>
@@ -881,301 +878,406 @@
     <col min="33" max="33" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+    </row>
+    <row r="2" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="9"/>
+      <c r="C2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="16"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
     </row>
-    <row r="2" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="9"/>
+      <c r="C3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+    </row>
+    <row r="4" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+    </row>
+    <row r="5" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="9" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="9" t="s">
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="9" t="s">
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="9" t="s">
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AA5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="9" t="s">
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AF5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="2" t="s">
+    <row r="6" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="2" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="2" t="s">
+      <c r="P6" s="10"/>
+      <c r="Q6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="10"/>
-      <c r="V3" s="2" t="s">
+      <c r="U6" s="10"/>
+      <c r="V6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Y6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="3" t="s">
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AC6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AD6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
     </row>
-    <row r="4" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="7" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D7" s="6">
         <v>4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E7" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F7" s="5">
         <v>6</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G7" s="5">
         <v>7</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H7" s="5">
         <v>8</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I7" s="5">
         <v>9</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J7" s="5">
         <v>10</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K7" s="5">
         <v>11</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L7" s="5">
         <v>12</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M7" s="5">
         <v>13</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N7" s="5">
         <v>14</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O7" s="5">
         <v>15</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P7" s="5">
         <v>16</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q7" s="5">
         <v>17</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R7" s="7">
         <v>18</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S7" s="7">
         <v>19</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T7" s="5">
         <v>20</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U7" s="5">
         <v>21</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V7" s="5">
         <v>22</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W7" s="5">
         <v>23</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X7" s="5">
         <v>24</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y7" s="5">
         <v>25</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z7" s="5">
         <v>26</v>
       </c>
-      <c r="AA4" s="7">
+      <c r="AA7" s="7">
         <v>27</v>
       </c>
-      <c r="AB4" s="8">
+      <c r="AB7" s="8">
         <v>28</v>
       </c>
-      <c r="AC4" s="5">
+      <c r="AC7" s="5">
         <v>29</v>
       </c>
-      <c r="AD4" s="5">
+      <c r="AD7" s="5">
         <v>30</v>
       </c>
-      <c r="AE4" s="5">
+      <c r="AE7" s="5">
         <v>31</v>
       </c>
-      <c r="AF4" s="5">
+      <c r="AF7" s="5">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="A1:AF1"/>
+  <mergeCells count="13">
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ttd report rekap golongan (kurang monitoring)
</commit_message>
<xml_diff>
--- a/templates/report/golongan.xlsx
+++ b/templates/report/golongan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64new\www\mojokerto_simpeg\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0CD046-ECBF-4273-A136-7FA94405E578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5DA219-A45C-4FAB-8824-99760CE12663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,27 +313,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -350,44 +335,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -395,18 +353,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
@@ -423,32 +378,20 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,9 +415,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1004662</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>400050</xdr:rowOff>
+      <xdr:colOff>2357212</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="464491" cy="552450"/>
     <xdr:pic>
@@ -504,7 +447,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1309462" y="400050"/>
+          <a:off x="2662012" y="266700"/>
           <a:ext cx="464491" cy="552450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -841,7 +784,7 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -879,155 +822,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
     </row>
     <row r="2" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="9"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
     </row>
     <row r="3" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="9"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
     </row>
     <row r="4" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
     </row>
     <row r="5" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="12"/>
@@ -1036,227 +979,227 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14" t="s">
+      <c r="J5" s="12"/>
+      <c r="K5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="14" t="s">
+      <c r="O5" s="12"/>
+      <c r="P5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="14" t="s">
+      <c r="T5" s="12"/>
+      <c r="U5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="V5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="14" t="s">
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="14" t="s">
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="AF5" s="14" t="s">
+      <c r="AF5" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="2" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="2" t="s">
+      <c r="P6" s="11"/>
+      <c r="Q6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="10"/>
-      <c r="V6" s="2" t="s">
+      <c r="U6" s="11"/>
+      <c r="V6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="W6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="X6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="3" t="s">
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AC6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AD6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
     </row>
     <row r="7" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>5</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>6</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>7</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>8</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>9</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>10</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>11</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>12</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>13</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>14</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <v>15</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="4">
         <v>16</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="4">
         <v>17</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="6">
         <v>18</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="6">
         <v>19</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="4">
         <v>20</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="4">
         <v>21</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="4">
         <v>22</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="4">
         <v>23</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7" s="4">
         <v>24</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="Y7" s="4">
         <v>25</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="4">
         <v>26</v>
       </c>
-      <c r="AA7" s="7">
+      <c r="AA7" s="6">
         <v>27</v>
       </c>
-      <c r="AB7" s="8">
+      <c r="AB7" s="7">
         <v>28</v>
       </c>
-      <c r="AC7" s="5">
+      <c r="AC7" s="4">
         <v>29</v>
       </c>
-      <c r="AD7" s="5">
+      <c r="AD7" s="4">
         <v>30</v>
       </c>
-      <c r="AE7" s="5">
+      <c r="AE7" s="4">
         <v>31</v>
       </c>
-      <c r="AF7" s="5">
+      <c r="AF7" s="4">
         <v>32</v>
       </c>
     </row>

</xml_diff>